<commit_message>
data succesfuly saved into exel from database
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -31,16 +31,31 @@
     <t>bahodur</t>
   </si>
   <si>
+    <t>1234</t>
+  </si>
+  <si>
     <t>emaff@gmail.com</t>
   </si>
   <si>
-    <t>1234</t>
-  </si>
-  <si>
     <t>nazarov</t>
   </si>
   <si>
     <t>emwewaff@gmail.com</t>
+  </si>
+  <si>
+    <t>Rakhim</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>rahimadv@gmail.com</t>
+  </si>
+  <si>
+    <t>Wed Mar 15 10:51:12 2023</t>
+  </si>
+  <si>
+    <t>Wed Mar 15 10:54:40 2023</t>
   </si>
 </sst>
 </file>
@@ -77,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,17 +115,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -389,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView tabSelected="true" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,10 +427,17 @@
     <col max="2" min="1" style="1" width="9.140625"/>
     <col customWidth="true" max="3" min="3" style="1" width="12.42578125"/>
     <col customWidth="true" max="4" min="4" style="1" width="25.140625"/>
-    <col customWidth="true" max="5" min="5" style="1" width="15.7109375"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" style="1" width="22"/>
     <col max="16384" min="6" style="1" width="9.140625"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
     <row r="2" spans="2:5">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -420,29 +454,45 @@
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="2"/>
@@ -451,6 +501,9 @@
       <c r="E6" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>